<commit_message>
Se suben compoenents para la parte de precentacion.
</commit_message>
<xml_diff>
--- a/CreditosFiscales/Documentacion/Desarrollo/Paquetes/CZCC24___FP_/CZCC24___FP_.xlsx
+++ b/CreditosFiscales/Documentacion/Desarrollo/Paquetes/CZCC24___FP_/CZCC24___FP_.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CredFiscales\CreditosFiscales\Documentacion\Desarrollo\Paquetes\CZCC24___FP_\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CA69A6-C934-47B4-8C4E-210CCA08864B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE83FC0-CA3D-4DC1-A27A-D8C5F6D8C15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="60" windowWidth="20400" windowHeight="10845" tabRatio="644" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45" yWindow="60" windowWidth="20400" windowHeight="10845" tabRatio="644" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instrucciones" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Instalables" sheetId="1" r:id="rId3"/>
     <sheet name="Componentes" sheetId="2" r:id="rId4"/>
     <sheet name="Firmas Conformidad" sheetId="6" r:id="rId5"/>
-    <sheet name="Encabezado" sheetId="5" state="hidden" r:id="rId6"/>
+    <sheet name="Encabezado" sheetId="5" r:id="rId6"/>
     <sheet name="tmp" sheetId="3" state="hidden" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="103">
   <si>
     <t>INSTALABLE</t>
   </si>
@@ -1009,6 +1009,131 @@
 01/11/2021</t>
   </si>
   <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>https://gitlab.sat.gob.mx/avl/cobranza_creditos_fiscales/tree/master/CODIGO/RCOBRANZA_ADEUDOS</t>
+  </si>
+  <si>
+    <t>Sat.CreditosFiscales.Procesamiento.Servicios.dll</t>
+  </si>
+  <si>
+    <t>Sat.CreditosFiscales.Comunes.Herramientas.dll</t>
+  </si>
+  <si>
+    <t>Sat.CreditosFiscales.Comunes.Entidades.dll</t>
+  </si>
+  <si>
+    <t>Sat.CreditosFiscales.Procesamiento.LogicaNegocio.dll</t>
+  </si>
+  <si>
+    <t>Sat.CreditosFiscales.Datos.AccesoDatos.dll</t>
+  </si>
+  <si>
+    <t>Jorge Abel Bolaños Nila</t>
+  </si>
+  <si>
+    <t>Arturo Efrain Mingues Alcantara</t>
+  </si>
+  <si>
+    <t>miaa677p</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Para descargar el código "Visor" en la siguiente ruta:
+* </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>https://gitlab.sat.gob.mx/avl/cobranza_creditos_fiscales/tree/master/CODIGO/RCOBRANZA_ADEUDOS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> ID/VERSIONAMIENTO:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>b2f05f843e</t>
+    </r>
+  </si>
+  <si>
+    <t>Creación del documento.</t>
+  </si>
+  <si>
+    <t>Angel Ramírez Mancera</t>
+  </si>
+  <si>
+    <t>Alejandro Dominguez Subias</t>
+  </si>
+  <si>
+    <t>José Ignacio García Carreño</t>
+  </si>
+  <si>
+    <t>Liberaciones SDMA-6</t>
+  </si>
+  <si>
+    <t>Lider Tecnico SDMA-6</t>
+  </si>
+  <si>
+    <t>José Eduardo Gutiérrez Delgado</t>
+  </si>
+  <si>
+    <t>Subadministrador de Proyectos Especificos (RAPE CBZ)</t>
+  </si>
+  <si>
+    <t>03_644_MAC_SitioWeb.docx</t>
+  </si>
+  <si>
+    <t>03_644_MAI_SitioWeb.docx</t>
+  </si>
+  <si>
+    <t>RMA INCS00000</t>
+  </si>
+  <si>
+    <t>https://gitlab.sat.gob.mx/avl/cobranza_creditos_fiscales/tree/master/DOCUMENTOS/rma_?????</t>
+  </si>
+  <si>
+    <t>Sat.CreditosFiscales.Presentacion.Herramientas.dll</t>
+  </si>
+  <si>
+    <t>Sat.CreditosFiscales.Presentacion.Portal.dll</t>
+  </si>
+  <si>
+    <t>CreditosLogEvento.cshtml</t>
+  </si>
+  <si>
+    <t>CreditosPeticion.cshtml</t>
+  </si>
+  <si>
+    <t>TemplateLogEvento.cshtml</t>
+  </si>
+  <si>
+    <t>TraductorBitacora.cshtml</t>
+  </si>
+  <si>
+    <t>TraductorLogEvento.cshtml</t>
+  </si>
+  <si>
+    <t>C:\CreFisCob\bin</t>
+  </si>
+  <si>
+    <t>C:\CreFisCob\Views\LogEventos</t>
+  </si>
+  <si>
+    <t>ENVIAR A LAS NUBE-SSO TQAGRPROMIIS03, TQAGRPROMIIS04 (PRODUCCION)</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -1026,7 +1151,7 @@
         <rFont val="Montserrat"/>
       </rPr>
       <t xml:space="preserve">
-CZCC24153DP_.xlsx</t>
+CZCC24___FP_.xlsx</t>
     </r>
   </si>
   <si>
@@ -1046,136 +1171,8 @@
         <rFont val="Montserrat"/>
       </rPr>
       <t xml:space="preserve">
-CZCC24153DP_.xlsx</t>
-    </r>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>https://gitlab.sat.gob.mx/avl/cobranza_creditos_fiscales/tree/master/CODIGO/RCOBRANZA_ADEUDOS</t>
-  </si>
-  <si>
-    <t>https://gitlab.sat.gob.mx/avl/cobranza_creditos_fiscales/tree/master/DOCUMENTOS/Id_8241</t>
-  </si>
-  <si>
-    <t>Sat.CreditosFiscales.Procesamiento.Servicios.dll</t>
-  </si>
-  <si>
-    <t>Sat.CreditosFiscales.Comunes.Herramientas.dll</t>
-  </si>
-  <si>
-    <t>Sat.CreditosFiscales.Comunes.Entidades.dll</t>
-  </si>
-  <si>
-    <t>Sat.CreditosFiscales.Procesamiento.LogicaNegocio.dll</t>
-  </si>
-  <si>
-    <t>Sat.CreditosFiscales.Datos.AccesoDatos.dll</t>
-  </si>
-  <si>
-    <t>Jorge Abel Bolaños Nila</t>
-  </si>
-  <si>
-    <t>Arturo Efrain Mingues Alcantara</t>
-  </si>
-  <si>
-    <t>miaa677p</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Para descargar el código "Visor" en la siguiente ruta:
-* </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>https://gitlab.sat.gob.mx/avl/cobranza_creditos_fiscales/tree/master/CODIGO/RCOBRANZA_ADEUDOS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve"> ID/VERSIONAMIENTO:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>b2f05f843e</t>
-    </r>
-  </si>
-  <si>
-    <t>Creación del documento.</t>
-  </si>
-  <si>
-    <t>Angel Ramírez Mancera</t>
-  </si>
-  <si>
-    <t>ENVIAR A LAS NUBE-SSO TQAGRPROMNET01, TQAGRPROMNET02, TQAGRPROMNET03 (PRODUCCION)</t>
-  </si>
-  <si>
-    <t>Alejandro Dominguez Subias</t>
-  </si>
-  <si>
-    <t>José Ignacio García Carreño</t>
-  </si>
-  <si>
-    <t>Liberaciones SDMA-6</t>
-  </si>
-  <si>
-    <t>Lider Tecnico SDMA-6</t>
-  </si>
-  <si>
-    <t>José Eduardo Gutiérrez Delgado</t>
-  </si>
-  <si>
-    <t>Subadministrador de Proyectos Especificos (RAPE CBZ)</t>
-  </si>
-  <si>
-    <t>03_644_MAC_SitioWeb.docx</t>
-  </si>
-  <si>
-    <t>03_644_MAI_SitioWeb.docx</t>
-  </si>
-  <si>
-    <t>RMA INCS00000</t>
-  </si>
-  <si>
-    <t>https://gitlab.sat.gob.mx/avl/cobranza_creditos_fiscales/tree/master/DOCUMENTOS/rma_?????</t>
-  </si>
-  <si>
-    <t>Sat.CreditosFiscales.Presentacion.Herramientas.dll</t>
-  </si>
-  <si>
-    <t>Sat.CreditosFiscales.Presentacion.Portal.dll</t>
-  </si>
-  <si>
-    <t>CreditosLogEvento.cshtml</t>
-  </si>
-  <si>
-    <t>CreditosPeticion.cshtml</t>
-  </si>
-  <si>
-    <t>TemplateLogEvento.cshtml</t>
-  </si>
-  <si>
-    <t>TraductorBitacora.cshtml</t>
-  </si>
-  <si>
-    <t>TraductorLogEvento.cshtml</t>
-  </si>
-  <si>
-    <t>C:\CreFisCob\bin</t>
-  </si>
-  <si>
-    <t>C:\CreFisCob\Views\LogEventos</t>
+CZCC24___FP_.xlsx</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2512,6 +2509,39 @@
     <xf numFmtId="0" fontId="14" fillId="11" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="57" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="54" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -2535,39 +2565,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="57" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2943,7 +2940,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Encabezado!$C$3:$K$7" spid="_x0000_s1143"/>
+                  <a14:cameraTool cellRange="Encabezado!$C$3:$K$7" spid="_x0000_s1153"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -3013,7 +3010,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Encabezado!$C$11:$K$16" spid="_x0000_s5239"/>
+                  <a14:cameraTool cellRange="Encabezado!$C$11:$K$16" spid="_x0000_s5249"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -3083,7 +3080,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Encabezado!$C$11:$K$16" spid="_x0000_s3186"/>
+                  <a14:cameraTool cellRange="Encabezado!$C$11:$K$16" spid="_x0000_s3196"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -3153,7 +3150,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Encabezado!$C$11:$K$16" spid="_x0000_s2165"/>
+                  <a14:cameraTool cellRange="Encabezado!$C$11:$K$16" spid="_x0000_s2175"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -4029,10 +4026,10 @@
         <v>1</v>
       </c>
       <c r="D15" s="58" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E15" s="59" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F15" s="60">
         <v>45392</v>
@@ -4062,8 +4059,8 @@
   </sheetPr>
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4079,59 +4076,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="109"/>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
-      <c r="I1" s="110"/>
+      <c r="A1" s="120"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="121"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="111"/>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="112"/>
+      <c r="A2" s="122"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="111"/>
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
-      <c r="H3" s="112"/>
-      <c r="I3" s="112"/>
+      <c r="A3" s="122"/>
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="123"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="111"/>
-      <c r="B4" s="112"/>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
-      <c r="G4" s="112"/>
-      <c r="H4" s="112"/>
-      <c r="I4" s="112"/>
+      <c r="A4" s="122"/>
+      <c r="B4" s="123"/>
+      <c r="C4" s="123"/>
+      <c r="D4" s="123"/>
+      <c r="E4" s="123"/>
+      <c r="F4" s="123"/>
+      <c r="G4" s="123"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="123"/>
     </row>
     <row r="5" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="111"/>
-      <c r="B5" s="112"/>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
-      <c r="F5" s="112"/>
-      <c r="G5" s="112"/>
-      <c r="H5" s="112"/>
-      <c r="I5" s="112"/>
+      <c r="A5" s="122"/>
+      <c r="B5" s="123"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="123"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="123"/>
+      <c r="H5" s="123"/>
+      <c r="I5" s="123"/>
     </row>
     <row r="6" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
@@ -4145,17 +4142,17 @@
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="A7" s="108" t="s">
+      <c r="A7" s="119" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="108"/>
-      <c r="C7" s="108"/>
-      <c r="D7" s="108"/>
-      <c r="E7" s="108"/>
-      <c r="F7" s="108"/>
-      <c r="G7" s="108"/>
-      <c r="H7" s="108"/>
-      <c r="I7" s="108"/>
+      <c r="B7" s="119"/>
+      <c r="C7" s="119"/>
+      <c r="D7" s="119"/>
+      <c r="E7" s="119"/>
+      <c r="F7" s="119"/>
+      <c r="G7" s="119"/>
+      <c r="H7" s="119"/>
+      <c r="I7" s="119"/>
     </row>
     <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" s="42"/>
@@ -4169,19 +4166,19 @@
       <c r="I8" s="42"/>
     </row>
     <row r="9" spans="1:9" s="43" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="118" t="s">
+      <c r="A9" s="110" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="119"/>
-      <c r="C9" s="120"/>
-      <c r="D9" s="116" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" s="117"/>
-      <c r="F9" s="117"/>
-      <c r="G9" s="117"/>
-      <c r="H9" s="117"/>
-      <c r="I9" s="117"/>
+      <c r="B9" s="111"/>
+      <c r="C9" s="112"/>
+      <c r="D9" s="108" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="109"/>
+      <c r="F9" s="109"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="109"/>
     </row>
     <row r="10" spans="1:9" s="43" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
@@ -4202,246 +4199,246 @@
       <c r="F10" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="115" t="s">
+      <c r="G10" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="115"/>
-      <c r="I10" s="115"/>
+      <c r="H10" s="107"/>
+      <c r="I10" s="107"/>
     </row>
     <row r="11" spans="1:9" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="52" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B11" s="53" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C11" s="54"/>
       <c r="D11" s="55"/>
       <c r="E11" s="55"/>
       <c r="F11" s="55"/>
-      <c r="G11" s="121" t="s">
-        <v>94</v>
-      </c>
-      <c r="H11" s="122"/>
-      <c r="I11" s="123"/>
+      <c r="G11" s="113" t="s">
+        <v>90</v>
+      </c>
+      <c r="H11" s="114"/>
+      <c r="I11" s="115"/>
     </row>
     <row r="12" spans="1:9" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" s="56" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B12" s="48" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C12" s="49"/>
       <c r="D12" s="50" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E12" s="50"/>
       <c r="F12" s="50"/>
-      <c r="G12" s="105" t="s">
-        <v>71</v>
-      </c>
-      <c r="H12" s="106"/>
-      <c r="I12" s="107"/>
+      <c r="G12" s="116" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" s="117"/>
+      <c r="I12" s="118"/>
     </row>
     <row r="13" spans="1:9" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="57" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B13" s="48" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C13" s="49"/>
       <c r="D13" s="50" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E13" s="50"/>
       <c r="F13" s="50"/>
-      <c r="G13" s="105" t="s">
-        <v>71</v>
-      </c>
-      <c r="H13" s="106"/>
-      <c r="I13" s="107"/>
+      <c r="G13" s="116" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" s="117"/>
+      <c r="I13" s="118"/>
     </row>
     <row r="14" spans="1:9" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="57" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B14" s="48" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C14" s="49"/>
       <c r="D14" s="50" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E14" s="50"/>
       <c r="F14" s="50"/>
-      <c r="G14" s="105" t="s">
-        <v>71</v>
-      </c>
-      <c r="H14" s="106"/>
-      <c r="I14" s="107"/>
+      <c r="G14" s="116" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" s="117"/>
+      <c r="I14" s="118"/>
     </row>
     <row r="15" spans="1:9" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="57" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B15" s="48" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C15" s="49"/>
       <c r="D15" s="50" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E15" s="50"/>
       <c r="F15" s="50"/>
-      <c r="G15" s="105" t="s">
-        <v>71</v>
-      </c>
-      <c r="H15" s="106"/>
-      <c r="I15" s="107"/>
+      <c r="G15" s="116" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="117"/>
+      <c r="I15" s="118"/>
     </row>
     <row r="16" spans="1:9" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="57" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B16" s="48" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C16" s="49"/>
       <c r="D16" s="50" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E16" s="50"/>
       <c r="F16" s="50"/>
-      <c r="G16" s="105" t="s">
-        <v>71</v>
-      </c>
-      <c r="H16" s="106"/>
-      <c r="I16" s="107"/>
+      <c r="G16" s="116" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16" s="117"/>
+      <c r="I16" s="118"/>
     </row>
     <row r="17" spans="1:9" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="57" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B17" s="48" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C17" s="49"/>
       <c r="D17" s="50" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E17" s="50"/>
       <c r="F17" s="50"/>
-      <c r="G17" s="105" t="s">
-        <v>71</v>
-      </c>
-      <c r="H17" s="106"/>
-      <c r="I17" s="107"/>
+      <c r="G17" s="116" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" s="117"/>
+      <c r="I17" s="118"/>
     </row>
     <row r="18" spans="1:9" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="57" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B18" s="48" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C18" s="49"/>
       <c r="D18" s="50" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E18" s="50"/>
       <c r="F18" s="50"/>
-      <c r="G18" s="105" t="s">
-        <v>71</v>
-      </c>
-      <c r="H18" s="106"/>
-      <c r="I18" s="107"/>
+      <c r="G18" s="116" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18" s="117"/>
+      <c r="I18" s="118"/>
     </row>
     <row r="19" spans="1:9" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="57" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B19" s="48" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C19" s="49"/>
       <c r="D19" s="50" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E19" s="50"/>
       <c r="F19" s="50"/>
-      <c r="G19" s="105"/>
-      <c r="H19" s="106"/>
-      <c r="I19" s="107"/>
+      <c r="G19" s="116"/>
+      <c r="H19" s="117"/>
+      <c r="I19" s="118"/>
     </row>
     <row r="20" spans="1:9" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="57" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B20" s="48" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C20" s="49"/>
       <c r="D20" s="50" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E20" s="50"/>
       <c r="F20" s="50"/>
-      <c r="G20" s="105"/>
-      <c r="H20" s="106"/>
-      <c r="I20" s="107"/>
+      <c r="G20" s="116"/>
+      <c r="H20" s="117"/>
+      <c r="I20" s="118"/>
     </row>
     <row r="21" spans="1:9" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="57" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B21" s="48" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C21" s="49"/>
       <c r="D21" s="50" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E21" s="50"/>
       <c r="F21" s="50"/>
-      <c r="G21" s="105"/>
-      <c r="H21" s="106"/>
-      <c r="I21" s="107"/>
+      <c r="G21" s="116"/>
+      <c r="H21" s="117"/>
+      <c r="I21" s="118"/>
     </row>
     <row r="22" spans="1:9" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="57" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B22" s="48" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C22" s="49"/>
       <c r="D22" s="50" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E22" s="50"/>
       <c r="F22" s="50"/>
-      <c r="G22" s="105"/>
-      <c r="H22" s="106"/>
-      <c r="I22" s="107"/>
+      <c r="G22" s="116"/>
+      <c r="H22" s="117"/>
+      <c r="I22" s="118"/>
     </row>
     <row r="23" spans="1:9" s="43" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="57" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B23" s="48" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C23" s="49"/>
       <c r="D23" s="50" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E23" s="50"/>
       <c r="F23" s="50"/>
-      <c r="G23" s="105"/>
-      <c r="H23" s="106"/>
-      <c r="I23" s="107"/>
+      <c r="G23" s="116"/>
+      <c r="H23" s="117"/>
+      <c r="I23" s="118"/>
     </row>
     <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A24" s="51"/>
@@ -4505,28 +4502,28 @@
       <c r="I28" s="14"/>
     </row>
     <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="A29" s="113" t="s">
+      <c r="A29" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="113"/>
-      <c r="C29" s="113"/>
-      <c r="D29" s="113"/>
-      <c r="E29" s="113"/>
-      <c r="F29" s="113"/>
-      <c r="G29" s="113"/>
-      <c r="H29" s="113"/>
-      <c r="I29" s="113"/>
+      <c r="B29" s="105"/>
+      <c r="C29" s="105"/>
+      <c r="D29" s="105"/>
+      <c r="E29" s="105"/>
+      <c r="F29" s="105"/>
+      <c r="G29" s="105"/>
+      <c r="H29" s="105"/>
+      <c r="I29" s="105"/>
     </row>
     <row r="30" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="114"/>
-      <c r="B30" s="114"/>
-      <c r="C30" s="114"/>
-      <c r="D30" s="114"/>
-      <c r="E30" s="114"/>
-      <c r="F30" s="114"/>
-      <c r="G30" s="114"/>
-      <c r="H30" s="114"/>
-      <c r="I30" s="114"/>
+      <c r="A30" s="106"/>
+      <c r="B30" s="106"/>
+      <c r="C30" s="106"/>
+      <c r="D30" s="106"/>
+      <c r="E30" s="106"/>
+      <c r="F30" s="106"/>
+      <c r="G30" s="106"/>
+      <c r="H30" s="106"/>
+      <c r="I30" s="106"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="8"/>
@@ -4560,16 +4557,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="A1:I5"/>
     <mergeCell ref="G16:I16"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="A1:I5"/>
     <mergeCell ref="A29:I29"/>
     <mergeCell ref="A30:I30"/>
     <mergeCell ref="G10:I10"/>
@@ -4580,6 +4572,11 @@
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="G14:I14"/>
     <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G20:I20"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -4607,8 +4604,8 @@
   </sheetPr>
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4623,52 +4620,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="112"/>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="112"/>
+      <c r="A1" s="123"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="123"/>
+      <c r="J1" s="123"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="112"/>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="112"/>
-      <c r="J2" s="112"/>
+      <c r="A2" s="123"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="112"/>
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
-      <c r="H3" s="112"/>
-      <c r="I3" s="112"/>
-      <c r="J3" s="112"/>
+      <c r="A3" s="123"/>
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="123"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
+      <c r="J3" s="123"/>
     </row>
     <row r="4" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="112"/>
-      <c r="B4" s="112"/>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
-      <c r="G4" s="112"/>
-      <c r="H4" s="112"/>
-      <c r="I4" s="112"/>
-      <c r="J4" s="112"/>
+      <c r="A4" s="123"/>
+      <c r="B4" s="123"/>
+      <c r="C4" s="123"/>
+      <c r="D4" s="123"/>
+      <c r="E4" s="123"/>
+      <c r="F4" s="123"/>
+      <c r="G4" s="123"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="123"/>
+      <c r="J4" s="123"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
@@ -4741,7 +4738,7 @@
       <c r="B10" s="124"/>
       <c r="C10" s="124"/>
       <c r="D10" s="126" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="E10" s="127"/>
       <c r="F10" s="127"/>
@@ -4781,13 +4778,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="149" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E13" s="150"/>
       <c r="F13" s="150"/>
@@ -4795,7 +4792,7 @@
         <v>6</v>
       </c>
       <c r="H13" s="149" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I13" s="150"/>
       <c r="J13" s="151"/>
@@ -4819,7 +4816,7 @@
       <c r="B15" s="152"/>
       <c r="C15" s="152"/>
       <c r="D15" s="153" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E15" s="153"/>
       <c r="F15" s="153"/>
@@ -4862,7 +4859,7 @@
     </row>
     <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" s="145" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B18" s="145"/>
       <c r="C18" s="145"/>
@@ -4904,7 +4901,7 @@
     </row>
     <row r="21" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="136" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B21" s="137"/>
       <c r="C21" s="137"/>
@@ -5179,14 +5176,14 @@
         <v>43</v>
       </c>
       <c r="C9" s="171" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D9" s="172"/>
       <c r="E9" s="37" t="s">
         <v>44</v>
       </c>
       <c r="F9" s="171" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G9" s="177"/>
       <c r="K9" s="32"/>
@@ -5197,14 +5194,14 @@
         <v>45</v>
       </c>
       <c r="C10" s="171" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D10" s="172"/>
       <c r="E10" s="37" t="s">
         <v>46</v>
       </c>
       <c r="F10" s="171" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G10" s="177"/>
       <c r="K10" s="32"/>
@@ -5262,7 +5259,7 @@
         <v>44</v>
       </c>
       <c r="C14" s="171" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D14" s="172"/>
       <c r="E14" s="37" t="s">
@@ -5278,7 +5275,7 @@
         <v>52</v>
       </c>
       <c r="C15" s="171" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D15" s="172"/>
       <c r="E15" s="37" t="s">
@@ -5359,7 +5356,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:I7"/>
+      <selection activeCell="E16" sqref="E16:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5435,7 +5432,7 @@
       </c>
       <c r="D7" s="199"/>
       <c r="E7" s="195" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="F7" s="196"/>
       <c r="G7" s="196"/>
@@ -5562,7 +5559,7 @@
       </c>
       <c r="D16" s="194"/>
       <c r="E16" s="195" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="F16" s="196"/>
       <c r="G16" s="196"/>

</xml_diff>